<commit_message>
user profiling files added
</commit_message>
<xml_diff>
--- a/Viraj/Utility Work/scenarios.xlsx
+++ b/Viraj/Utility Work/scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SLIIT\4th Year\Research\Python Work\Implementation\Utility Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SLIIT\4th Year\Research\Python Work\CodeFlexers-Initial-Implementation\Viraj\Utility Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
@@ -46,6 +46,18 @@
   <si>
     <t>Checked</t>
   </si>
+  <si>
+    <t>Gender_Preference</t>
+  </si>
+  <si>
+    <t>Tested</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
 </sst>
 </file>
 
@@ -61,22 +73,22 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +98,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -102,15 +120,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -386,263 +429,576 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="4" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I1:I2 H18:H1048576 H2:J17">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Tested">
+      <formula>NOT(ISERROR(SEARCH("Tested",H1)))</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:J17">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Problem">
+      <formula>NOT(ISERROR(SEARCH("Problem",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>